<commit_message>
Update ATP with morning tests
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Instructions</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Given that I'm signed in when I view the Home page then I can start a game by selecting a player listed on the Home page.</t>
+  </si>
+  <si>
+    <t>MTM 3/11</t>
   </si>
   <si>
     <t>Given that the player I selected isn't yet in a game when I select that player then the system will begin a checkers game and assign me as the starting (Red) player and my opponent as the White player.</t>
@@ -213,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -237,7 +240,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -256,13 +259,28 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -3899,11 +3917,15 @@
       <c r="B9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="17"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="14"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
@@ -3927,10 +3949,14 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="2"/>
       <c r="E10" s="10"/>
       <c r="F10" s="2"/>
       <c r="G10" s="10"/>
@@ -3957,10 +3983,14 @@
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="2"/>
       <c r="G11" s="10"/>
@@ -3987,10 +4017,14 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="10"/>
       <c r="F12" s="2"/>
       <c r="G12" s="10"/>
@@ -4017,7 +4051,7 @@
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="2"/>
@@ -4047,7 +4081,7 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="2"/>
@@ -4077,7 +4111,7 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="2"/>
@@ -4105,274 +4139,278 @@
       <c r="Z15" s="11"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="19"/>
-      <c r="W16" s="19"/>
-      <c r="X16" s="19"/>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="19"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="20" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19"/>
-      <c r="X17" s="19"/>
-      <c r="Y17" s="19"/>
-      <c r="Z17" s="19"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="21" t="s">
+      <c r="C16" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="21" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="21" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="21" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="21" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="21" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="26" t="s">
         <v>38</v>
       </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="29"/>
+      <c r="X23" s="29"/>
+      <c r="Y23" s="29"/>
+      <c r="Z23" s="29"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="15"/>
+      <c r="G24" s="17"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>

</xml_diff>

<commit_message>
Finalized ATP for Sprint 1
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>Instructions</t>
   </si>
@@ -110,6 +110,12 @@
     <t>Given a valid, initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>MTM 3/11 - Feature is pending implementation</t>
+  </si>
+  <si>
     <t>Given a valid, initial game board when I drag a piece to an occupied space then the piece should not be droppable.</t>
   </si>
   <si>
@@ -147,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -183,13 +189,24 @@
       <sz val="12.0"/>
       <color theme="1"/>
     </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -216,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -261,7 +278,7 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -269,6 +286,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -279,7 +299,7 @@
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -287,9 +307,6 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -302,9 +319,6 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
@@ -3954,7 +3968,7 @@
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="10"/>
@@ -3988,7 +4002,7 @@
       <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="10"/>
@@ -4022,7 +4036,7 @@
       <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="10"/>
@@ -4053,8 +4067,12 @@
       <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="E13" s="10"/>
       <c r="F13" s="2"/>
       <c r="G13" s="10"/>
@@ -4081,10 +4099,14 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="19" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="2"/>
       <c r="G14" s="10"/>
@@ -4111,10 +4133,14 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="2"/>
       <c r="E15" s="10"/>
       <c r="F15" s="2"/>
       <c r="G15" s="10"/>
@@ -4139,72 +4165,72 @@
       <c r="Z15" s="11"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20" t="s">
-        <v>31</v>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21" t="s">
+        <v>33</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="25" t="s">
-        <v>32</v>
+      <c r="A17" s="23" t="s">
+        <v>34</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
@@ -4234,7 +4260,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
@@ -4264,7 +4290,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="28"/>
@@ -4294,7 +4320,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="28"/>
@@ -4324,7 +4350,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
@@ -4354,7 +4380,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -4383,8 +4409,8 @@
       <c r="Z23" s="29"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="30" t="s">
-        <v>39</v>
+      <c r="A24" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="17"/>
@@ -4393,24 +4419,24 @@
       <c r="F24" s="14"/>
       <c r="G24" s="17"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="31"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="31"/>
-      <c r="Z24" s="31"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>

</xml_diff>

<commit_message>
ATP updated to include new issue found in the sign-in story
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>Instructions</t>
   </si>
@@ -80,6 +80,12 @@
     <t>Given that I am on the Sign-in page when I enter a name that does not contain at least one alphanumeric character or contains one or more characters that are not alphanumeric or spaces and click the Sign-in button then I expect the system to reject this name and return the Sign-in page.</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>MTM 3/11 - Non-alphanumeric characters are accepted</t>
+  </si>
+  <si>
     <t>Given that someone else with my name has signed-in when I enter my name in the Sign-in form  and click the Sign-in button then I expect the system to reject my sign-in and return the Sign-in page for me to try a different name.</t>
   </si>
   <si>
@@ -108,9 +114,6 @@
   </si>
   <si>
     <t>Given a valid, initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>MTM 3/11 - Feature is pending implementation</t>
@@ -153,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -184,6 +187,12 @@
       <sz val="11.0"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -233,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -269,6 +278,12 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -284,10 +299,7 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3793,11 +3805,11 @@
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>14</v>
+      <c r="C5" s="13" t="s">
+        <v>19</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>15</v>
+      <c r="D5" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="2"/>
@@ -3825,7 +3837,7 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>14</v>
@@ -3859,7 +3871,7 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>14</v>
@@ -3893,7 +3905,7 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>14</v>
@@ -3925,22 +3937,22 @@
       <c r="Z8" s="11"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
-        <v>22</v>
+      <c r="A9" s="15" t="s">
+        <v>24</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>23</v>
+      <c r="B9" s="16" t="s">
+        <v>25</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>24</v>
+      <c r="D9" s="18" t="s">
+        <v>26</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="14"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
@@ -3963,13 +3975,13 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="2"/>
@@ -3997,13 +4009,13 @@
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="2"/>
@@ -4031,13 +4043,13 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="2"/>
@@ -4065,13 +4077,13 @@
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>30</v>
+      <c r="D13" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="2"/>
@@ -4099,13 +4111,13 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>30</v>
+      <c r="D14" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="2"/>
@@ -4133,13 +4145,13 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>30</v>
+      <c r="D15" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="2"/>
@@ -4165,278 +4177,278 @@
       <c r="Z15" s="11"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21" t="s">
-        <v>33</v>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22" t="s">
+        <v>34</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>24</v>
+      <c r="D16" s="24" t="s">
+        <v>26</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="25"/>
-      <c r="U16" s="25"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="26"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="25"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="26" t="s">
+      <c r="A17" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-      <c r="W18" s="29"/>
-      <c r="X18" s="29"/>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="29"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="26" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="29"/>
-      <c r="Z19" s="29"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="29"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="26" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="30"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
-      <c r="X21" s="29"/>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="26" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="30"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="29"/>
-      <c r="W22" s="29"/>
-      <c r="X22" s="29"/>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="29"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="26" t="s">
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="30"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
-      <c r="T23" s="29"/>
-      <c r="U23" s="29"/>
-      <c r="V23" s="29"/>
-      <c r="W23" s="29"/>
-      <c r="X23" s="29"/>
-      <c r="Y23" s="29"/>
-      <c r="Z23" s="29"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="16" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="30"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="30"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="30"/>
-      <c r="Z24" s="30"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
+      <c r="Z23" s="30"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>

</xml_diff>